<commit_message>
improved save, improved combat, added gulden loot
</commit_message>
<xml_diff>
--- a/Combat/Game_Data.xlsx
+++ b/Combat/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -17,18 +17,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Level</t>
-  </si>
-  <si>
-    <t>Experience</t>
   </si>
   <si>
     <t>Strength</t>
   </si>
   <si>
     <t>Defense</t>
+  </si>
+  <si>
+    <t>Total Experience</t>
+  </si>
+  <si>
+    <t>Incremental Experience</t>
+  </si>
+  <si>
+    <t>Enemies at Level</t>
+  </si>
+  <si>
+    <t>Experience Per Enemy</t>
+  </si>
+  <si>
+    <t>Change in Incremental</t>
   </si>
 </sst>
 </file>
@@ -381,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E103"/>
+  <dimension ref="A2:H103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -393,21 +405,35 @@
     <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.77734375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="20.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -419,11 +445,12 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1">
+        <f>B3+E4</f>
         <v>10000</v>
       </c>
       <c r="C4" s="1">
@@ -434,1688 +461,3084 @@
         <f>B3*0.1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1">
+        <f>E4/G4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <f>B4+D5</f>
+        <f t="shared" ref="B5:B68" si="0">B4+E5</f>
         <v>21000</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C68" si="0">C4+$C$2</f>
+        <f t="shared" ref="C5:C68" si="1">C4+$C$2</f>
         <v>20000</v>
       </c>
       <c r="D5" s="1">
         <f>B4*1.1</f>
         <v>11000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <f>E4+F5</f>
+        <v>11000</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H68" si="2">E5/G5</f>
+        <v>91.666666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B68" si="1">C6+D6</f>
-        <v>53100</v>
+        <f t="shared" si="0"/>
+        <v>34000</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30000</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:D69" si="2">B5*1.1</f>
+        <f t="shared" ref="D6:D69" si="3">B5*1.1</f>
         <v>23100.000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E69" si="4">E5+F6</f>
+        <v>13000</v>
+      </c>
+      <c r="F6">
+        <v>2000</v>
+      </c>
+      <c r="G6">
+        <v>140</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>92.857142857142861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>98410</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
         <v>40000</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="2"/>
-        <v>58410.000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>37400</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="4"/>
+        <v>16000</v>
+      </c>
+      <c r="F7">
+        <v>3000</v>
+      </c>
+      <c r="G7">
+        <v>160</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <f>C8+D8</f>
-        <v>158251</v>
+        <f t="shared" si="0"/>
+        <v>70000</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50000</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="2"/>
-        <v>108251.00000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>55000.000000000007</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="4"/>
+        <v>20000</v>
+      </c>
+      <c r="F8">
+        <v>4000</v>
+      </c>
+      <c r="G8">
+        <v>180</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>111.11111111111111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>95000</v>
+      </c>
+      <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>234076.1</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
         <v>60000</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="2"/>
-        <v>174076.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>77000</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="4"/>
+        <v>25000</v>
+      </c>
+      <c r="F9">
+        <v>5000</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>126000</v>
+      </c>
+      <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>327483.71000000002</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="2"/>
-        <v>257483.71000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>104500.00000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="4"/>
+        <v>31000</v>
+      </c>
+      <c r="F10">
+        <v>6000</v>
+      </c>
+      <c r="G10">
+        <v>220</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>140.90909090909091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>440232.08100000006</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="0"/>
         <v>80000</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
-        <v>360232.08100000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>138600</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="4"/>
+        <v>38000</v>
+      </c>
+      <c r="F11">
+        <v>7000</v>
+      </c>
+      <c r="G11">
+        <v>240</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>158.33333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>210000</v>
+      </c>
+      <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>574255.28910000017</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
         <v>90000</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="2"/>
-        <v>484255.28910000011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>180400.00000000003</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="4"/>
+        <v>46000</v>
+      </c>
+      <c r="F12">
+        <v>8000</v>
+      </c>
+      <c r="G12">
+        <v>260</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>176.92307692307693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>265000</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>731680.81801000028</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
-        <v>631680.81801000028</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>231000.00000000003</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="4"/>
+        <v>55000</v>
+      </c>
+      <c r="F13">
+        <v>9000</v>
+      </c>
+      <c r="G13">
+        <v>280</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>196.42857142857142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="1"/>
-        <v>914848.89981100033</v>
+        <f t="shared" si="0"/>
+        <v>330000</v>
       </c>
       <c r="C14" s="1">
         <f>C13+$C$2</f>
         <v>110000</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="2"/>
-        <v>804848.89981100033</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>291500</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="4"/>
+        <v>65000</v>
+      </c>
+      <c r="F14">
+        <v>10000</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>216.66666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>406000</v>
+      </c>
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>1126333.7897921004</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="0"/>
         <v>120000</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
-        <v>1006333.7897921004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>363000.00000000006</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="4"/>
+        <v>76000</v>
+      </c>
+      <c r="F15">
+        <v>11000</v>
+      </c>
+      <c r="G15">
+        <v>320</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>237.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>494000</v>
+      </c>
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>1368967.1687713105</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
         <v>130000</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="2"/>
-        <v>1238967.1687713105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>446600.00000000006</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="4"/>
+        <v>88000</v>
+      </c>
+      <c r="F16">
+        <v>12000</v>
+      </c>
+      <c r="G16">
+        <v>340</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>258.8235294117647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>595000</v>
+      </c>
+      <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>1645863.8856484417</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="0"/>
         <v>140000</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
-        <v>1505863.8856484417</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>543400</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="4"/>
+        <v>101000</v>
+      </c>
+      <c r="F17">
+        <v>13000</v>
+      </c>
+      <c r="G17">
+        <v>360</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>280.55555555555554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>710000</v>
+      </c>
+      <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>1960450.2742132861</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="0"/>
         <v>150000</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
-        <v>1810450.2742132861</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>654500</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="4"/>
+        <v>115000</v>
+      </c>
+      <c r="F18">
+        <v>14000</v>
+      </c>
+      <c r="G18">
+        <v>380</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>302.63157894736844</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>840000</v>
+      </c>
+      <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>2316495.3016346148</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="0"/>
         <v>160000</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="2"/>
-        <v>2156495.3016346148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>781000.00000000012</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="4"/>
+        <v>130000</v>
+      </c>
+      <c r="F19">
+        <v>15000</v>
+      </c>
+      <c r="G19">
+        <v>400</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>986000</v>
+      </c>
+      <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>2718144.8317980766</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="0"/>
         <v>170000</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="2"/>
-        <v>2548144.8317980766</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>924000.00000000012</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="4"/>
+        <v>146000</v>
+      </c>
+      <c r="F20">
+        <v>16000</v>
+      </c>
+      <c r="G20">
+        <v>420</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>347.61904761904759</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>1149000</v>
+      </c>
+      <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>3169959.3149778848</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" si="0"/>
         <v>180000</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
-        <v>2989959.3149778848</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1084600</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="4"/>
+        <v>163000</v>
+      </c>
+      <c r="F21">
+        <v>17000</v>
+      </c>
+      <c r="G21">
+        <v>440</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>370.45454545454544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>1330000</v>
+      </c>
+      <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>3676955.2464756737</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="0"/>
         <v>190000</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="2"/>
-        <v>3486955.2464756737</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1263900</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="4"/>
+        <v>181000</v>
+      </c>
+      <c r="F22">
+        <v>18000</v>
+      </c>
+      <c r="G22">
+        <v>460</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>393.47826086956519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>1530000</v>
+      </c>
+      <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>4244650.7711232416</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="2"/>
-        <v>4044650.7711232416</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1463000.0000000002</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="F23">
+        <v>19000</v>
+      </c>
+      <c r="G23">
+        <v>480</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>416.66666666666669</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>1750000</v>
+      </c>
+      <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>4879115.8482355662</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="0"/>
         <v>210000</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
-        <v>4669115.8482355662</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1683000.0000000002</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="4"/>
+        <v>220000</v>
+      </c>
+      <c r="F24">
+        <v>20000</v>
+      </c>
+      <c r="G24">
+        <v>500</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>1991000</v>
+      </c>
+      <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>5587027.4330591233</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="0"/>
         <v>220000</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="2"/>
-        <v>5367027.4330591233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1925000.0000000002</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="4"/>
+        <v>241000</v>
+      </c>
+      <c r="F25">
+        <v>21000</v>
+      </c>
+      <c r="G25">
+        <v>520</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>463.46153846153845</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
       <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>2254000</v>
+      </c>
+      <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>6375730.1763650365</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="0"/>
         <v>230000</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="2"/>
-        <v>6145730.1763650365</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>2190100</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="4"/>
+        <v>263000</v>
+      </c>
+      <c r="F26">
+        <v>22000</v>
+      </c>
+      <c r="G26">
+        <v>540</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>487.03703703703701</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
       <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>2540000</v>
+      </c>
+      <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>7253303.1940015405</v>
-      </c>
-      <c r="C27" s="1">
-        <f t="shared" si="0"/>
         <v>240000</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="2"/>
-        <v>7013303.1940015405</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>2479400</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="4"/>
+        <v>286000</v>
+      </c>
+      <c r="F27">
+        <v>23000</v>
+      </c>
+      <c r="G27">
+        <v>560</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>510.71428571428572</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>2850000</v>
+      </c>
+      <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>8228633.5134016955</v>
-      </c>
-      <c r="C28" s="1">
-        <f t="shared" si="0"/>
         <v>250000</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="2"/>
-        <v>7978633.5134016955</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>2794000</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="4"/>
+        <v>310000</v>
+      </c>
+      <c r="F28">
+        <v>24000</v>
+      </c>
+      <c r="G28">
+        <v>580</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>534.48275862068965</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
       <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>3185000</v>
+      </c>
+      <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>9311496.8647418655</v>
-      </c>
-      <c r="C29" s="1">
-        <f t="shared" si="0"/>
         <v>260000</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="2"/>
-        <v>9051496.8647418655</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>3135000.0000000005</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="4"/>
+        <v>335000</v>
+      </c>
+      <c r="F29">
+        <v>25000</v>
+      </c>
+      <c r="G29">
+        <v>600</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="2"/>
+        <v>558.33333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
       <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>3546000</v>
+      </c>
+      <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>10512646.551216053</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="0"/>
         <v>270000</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="2"/>
-        <v>10242646.551216053</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>3503500.0000000005</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="4"/>
+        <v>361000</v>
+      </c>
+      <c r="F30">
+        <v>26000</v>
+      </c>
+      <c r="G30">
+        <v>620</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="2"/>
+        <v>582.25806451612902</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>3934000</v>
+      </c>
+      <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>11843911.206337659</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="0"/>
         <v>280000</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="2"/>
-        <v>11563911.206337659</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>3900600.0000000005</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="4"/>
+        <v>388000</v>
+      </c>
+      <c r="F31">
+        <v>27000</v>
+      </c>
+      <c r="G31">
+        <v>640</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="2"/>
+        <v>606.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>4350000</v>
+      </c>
+      <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>13318302.326971425</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="0"/>
         <v>290000</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="2"/>
-        <v>13028302.326971425</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>4327400</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="4"/>
+        <v>416000</v>
+      </c>
+      <c r="F32">
+        <v>28000</v>
+      </c>
+      <c r="G32">
+        <v>660</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="2"/>
+        <v>630.30303030303025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
       <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>4795000</v>
+      </c>
+      <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>14950132.559668569</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="2"/>
-        <v>14650132.559668569</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>4785000</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="4"/>
+        <v>445000</v>
+      </c>
+      <c r="F33">
+        <v>29000</v>
+      </c>
+      <c r="G33">
+        <v>680</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="2"/>
+        <v>654.41176470588232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
       <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>5270000</v>
+      </c>
+      <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>16755145.815635428</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" si="0"/>
         <v>310000</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="2"/>
-        <v>16445145.815635428</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>5274500</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="4"/>
+        <v>475000</v>
+      </c>
+      <c r="F34">
+        <v>30000</v>
+      </c>
+      <c r="G34">
+        <v>700</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="2"/>
+        <v>678.57142857142856</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
       <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>5776000</v>
+      </c>
+      <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>18750660.397198971</v>
-      </c>
-      <c r="C35" s="1">
-        <f t="shared" si="0"/>
         <v>320000</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="2"/>
-        <v>18430660.397198971</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>5797000.0000000009</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="4"/>
+        <v>506000</v>
+      </c>
+      <c r="F35">
+        <v>31000</v>
+      </c>
+      <c r="G35">
+        <v>720</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="2"/>
+        <v>702.77777777777783</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>6314000</v>
+      </c>
+      <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>20955726.43691887</v>
-      </c>
-      <c r="C36" s="1">
-        <f t="shared" si="0"/>
         <v>330000</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="2"/>
-        <v>20625726.43691887</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>6353600.0000000009</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="4"/>
+        <v>538000</v>
+      </c>
+      <c r="F36">
+        <v>32000</v>
+      </c>
+      <c r="G36">
+        <v>740</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="2"/>
+        <v>727.02702702702697</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
       <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>6885000</v>
+      </c>
+      <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>23391299.08061076</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="0"/>
         <v>340000</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="2"/>
-        <v>23051299.08061076</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>6945400.0000000009</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="4"/>
+        <v>571000</v>
+      </c>
+      <c r="F37">
+        <v>33000</v>
+      </c>
+      <c r="G37">
+        <v>760</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="2"/>
+        <v>751.31578947368416</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
       <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>7490000</v>
+      </c>
+      <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>26080428.988671839</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="0"/>
         <v>350000</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="2"/>
-        <v>25730428.988671839</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>7573500.0000000009</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="4"/>
+        <v>605000</v>
+      </c>
+      <c r="F38">
+        <v>34000</v>
+      </c>
+      <c r="G38">
+        <v>780</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="2"/>
+        <v>775.64102564102564</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
       <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>8130000</v>
+      </c>
+      <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>29048471.887539025</v>
-      </c>
-      <c r="C39" s="1">
-        <f t="shared" si="0"/>
         <v>360000</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="2"/>
-        <v>28688471.887539025</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>8239000.0000000009</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="4"/>
+        <v>640000</v>
+      </c>
+      <c r="F39">
+        <v>35000</v>
+      </c>
+      <c r="G39">
+        <v>800</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>8806000</v>
+      </c>
+      <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>32323319.076292932</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="0"/>
         <v>370000</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="2"/>
-        <v>31953319.076292932</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>8943000</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="4"/>
+        <v>676000</v>
+      </c>
+      <c r="F40">
+        <v>36000</v>
+      </c>
+      <c r="G40">
+        <v>820</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="2"/>
+        <v>824.39024390243901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
       <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>9519000</v>
+      </c>
+      <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>35935650.983922228</v>
-      </c>
-      <c r="C41" s="1">
-        <f t="shared" si="0"/>
         <v>380000</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="2"/>
-        <v>35555650.983922228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>9686600</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="4"/>
+        <v>713000</v>
+      </c>
+      <c r="F41">
+        <v>37000</v>
+      </c>
+      <c r="G41">
+        <v>840</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="2"/>
+        <v>848.80952380952385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
       <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>10270000</v>
+      </c>
+      <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>39919216.082314454</v>
-      </c>
-      <c r="C42" s="1">
-        <f t="shared" si="0"/>
         <v>390000</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="2"/>
-        <v>39529216.082314454</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>10470900</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="4"/>
+        <v>751000</v>
+      </c>
+      <c r="F42">
+        <v>38000</v>
+      </c>
+      <c r="G42">
+        <v>860</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="2"/>
+        <v>873.25581395348843</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
       <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>11060000</v>
+      </c>
+      <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>44311137.690545902</v>
-      </c>
-      <c r="C43" s="1">
-        <f t="shared" si="0"/>
         <v>400000</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="2"/>
-        <v>43911137.690545902</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>11297000</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="4"/>
+        <v>790000</v>
+      </c>
+      <c r="F43">
+        <v>39000</v>
+      </c>
+      <c r="G43">
+        <v>880</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="2"/>
+        <v>897.72727272727275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
       <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>11890000</v>
+      </c>
+      <c r="C44" s="1">
         <f t="shared" si="1"/>
-        <v>49152251.459600493</v>
-      </c>
-      <c r="C44" s="1">
-        <f t="shared" si="0"/>
         <v>410000</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="2"/>
-        <v>48742251.459600493</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>12166000.000000002</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="4"/>
+        <v>830000</v>
+      </c>
+      <c r="F44">
+        <v>40000</v>
+      </c>
+      <c r="G44">
+        <v>900</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="2"/>
+        <v>922.22222222222217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
       <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>12761000</v>
+      </c>
+      <c r="C45" s="1">
         <f t="shared" si="1"/>
-        <v>54487476.605560549</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" si="0"/>
         <v>420000</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="2"/>
-        <v>54067476.605560549</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>13079000.000000002</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="4"/>
+        <v>871000</v>
+      </c>
+      <c r="F45">
+        <v>41000</v>
+      </c>
+      <c r="G45">
+        <v>920</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="2"/>
+        <v>946.73913043478262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
       <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>13674000</v>
+      </c>
+      <c r="C46" s="1">
         <f t="shared" si="1"/>
-        <v>60366224.266116612</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" si="0"/>
         <v>430000</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="2"/>
-        <v>59936224.266116612</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>14037100.000000002</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="4"/>
+        <v>913000</v>
+      </c>
+      <c r="F46">
+        <v>42000</v>
+      </c>
+      <c r="G46">
+        <v>940</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="2"/>
+        <v>971.27659574468089</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
       <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>14630000</v>
+      </c>
+      <c r="C47" s="1">
         <f t="shared" si="1"/>
-        <v>66842846.692728281</v>
-      </c>
-      <c r="C47" s="1">
-        <f t="shared" si="0"/>
         <v>440000</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="2"/>
-        <v>66402846.692728281</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>15041400.000000002</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="4"/>
+        <v>956000</v>
+      </c>
+      <c r="F47">
+        <v>43000</v>
+      </c>
+      <c r="G47">
+        <v>960</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="2"/>
+        <v>995.83333333333337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
       <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>15630000</v>
+      </c>
+      <c r="C48" s="1">
         <f t="shared" si="1"/>
-        <v>73977131.362001121</v>
-      </c>
-      <c r="C48" s="1">
-        <f t="shared" si="0"/>
         <v>450000</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="2"/>
-        <v>73527131.362001121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>16093000.000000002</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="F48">
+        <v>44000</v>
+      </c>
+      <c r="G48">
+        <v>980</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="2"/>
+        <v>1020.4081632653061</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>16675000</v>
+      </c>
+      <c r="C49" s="1">
         <f t="shared" si="1"/>
-        <v>81834844.498201236</v>
-      </c>
-      <c r="C49" s="1">
-        <f t="shared" si="0"/>
         <v>460000</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="2"/>
-        <v>81374844.498201236</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>17193000</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="4"/>
+        <v>1045000</v>
+      </c>
+      <c r="F49">
+        <v>45000</v>
+      </c>
+      <c r="G49">
+        <v>1000</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="2"/>
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50" s="1">
+        <f t="shared" si="0"/>
+        <v>17766000</v>
+      </c>
+      <c r="C50" s="1">
         <f t="shared" si="1"/>
-        <v>90488328.948021367</v>
-      </c>
-      <c r="C50" s="1">
-        <f t="shared" si="0"/>
         <v>470000</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="2"/>
-        <v>90018328.948021367</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>18342500</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="4"/>
+        <v>1091000</v>
+      </c>
+      <c r="F50">
+        <v>46000</v>
+      </c>
+      <c r="G50">
+        <v>1020</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="2"/>
+        <v>1069.6078431372548</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51" s="1">
+        <f t="shared" si="0"/>
+        <v>18904000</v>
+      </c>
+      <c r="C51" s="1">
         <f t="shared" si="1"/>
-        <v>100017161.84282351</v>
-      </c>
-      <c r="C51" s="1">
-        <f t="shared" si="0"/>
         <v>480000</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="2"/>
-        <v>99537161.842823505</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>19542600</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="4"/>
+        <v>1138000</v>
+      </c>
+      <c r="F51">
+        <v>47000</v>
+      </c>
+      <c r="G51">
+        <v>1040</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="2"/>
+        <v>1094.2307692307693</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52" s="1">
+        <f t="shared" si="0"/>
+        <v>20090000</v>
+      </c>
+      <c r="C52" s="1">
         <f t="shared" si="1"/>
-        <v>110508878.02710587</v>
-      </c>
-      <c r="C52" s="1">
-        <f t="shared" si="0"/>
         <v>490000</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="2"/>
-        <v>110018878.02710587</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>20794400</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="4"/>
+        <v>1186000</v>
+      </c>
+      <c r="F52">
+        <v>48000</v>
+      </c>
+      <c r="G52">
+        <v>1060</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="2"/>
+        <v>1118.867924528302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53" s="1">
+        <f t="shared" si="0"/>
+        <v>21325000</v>
+      </c>
+      <c r="C53" s="1">
         <f t="shared" si="1"/>
-        <v>122059765.82981646</v>
-      </c>
-      <c r="C53" s="1">
-        <f t="shared" si="0"/>
         <v>500000</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="2"/>
-        <v>121559765.82981646</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>22099000</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="4"/>
+        <v>1235000</v>
+      </c>
+      <c r="F53">
+        <v>49000</v>
+      </c>
+      <c r="G53">
+        <v>1080</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="2"/>
+        <v>1143.5185185185185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>51</v>
       </c>
       <c r="B54" s="1">
+        <f t="shared" si="0"/>
+        <v>22610000</v>
+      </c>
+      <c r="C54" s="1">
         <f t="shared" si="1"/>
-        <v>134775742.41279811</v>
-      </c>
-      <c r="C54" s="1">
-        <f t="shared" si="0"/>
         <v>510000</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="2"/>
-        <v>134265742.41279811</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>23457500.000000004</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="4"/>
+        <v>1285000</v>
+      </c>
+      <c r="F54">
+        <v>50000</v>
+      </c>
+      <c r="G54">
+        <v>1100</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="2"/>
+        <v>1168.1818181818182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>52</v>
       </c>
       <c r="B55" s="1">
+        <f t="shared" si="0"/>
+        <v>23946000</v>
+      </c>
+      <c r="C55" s="1">
         <f t="shared" si="1"/>
-        <v>148773316.65407792</v>
-      </c>
-      <c r="C55" s="1">
-        <f t="shared" si="0"/>
         <v>520000</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="2"/>
-        <v>148253316.65407792</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>24871000.000000004</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="4"/>
+        <v>1336000</v>
+      </c>
+      <c r="F55">
+        <v>51000</v>
+      </c>
+      <c r="G55">
+        <v>1120</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="2"/>
+        <v>1192.8571428571429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>53</v>
       </c>
       <c r="B56" s="1">
+        <f t="shared" si="0"/>
+        <v>25334000</v>
+      </c>
+      <c r="C56" s="1">
         <f t="shared" si="1"/>
-        <v>164180648.31948572</v>
-      </c>
-      <c r="C56" s="1">
-        <f t="shared" si="0"/>
         <v>530000</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="2"/>
-        <v>163650648.31948572</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>26340600.000000004</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="4"/>
+        <v>1388000</v>
+      </c>
+      <c r="F56">
+        <v>52000</v>
+      </c>
+      <c r="G56">
+        <v>1140</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="2"/>
+        <v>1217.5438596491229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>54</v>
       </c>
       <c r="B57" s="1">
+        <f t="shared" si="0"/>
+        <v>26775000</v>
+      </c>
+      <c r="C57" s="1">
         <f t="shared" si="1"/>
-        <v>181138713.1514343</v>
-      </c>
-      <c r="C57" s="1">
-        <f t="shared" si="0"/>
         <v>540000</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="2"/>
-        <v>180598713.1514343</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>27867400.000000004</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="4"/>
+        <v>1441000</v>
+      </c>
+      <c r="F57">
+        <v>53000</v>
+      </c>
+      <c r="G57">
+        <v>1160</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="2"/>
+        <v>1242.2413793103449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" s="1">
+        <f t="shared" si="0"/>
+        <v>28270000</v>
+      </c>
+      <c r="C58" s="1">
         <f t="shared" si="1"/>
-        <v>199802584.46657774</v>
-      </c>
-      <c r="C58" s="1">
-        <f t="shared" si="0"/>
         <v>550000</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="2"/>
-        <v>199252584.46657774</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>29452500.000000004</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="4"/>
+        <v>1495000</v>
+      </c>
+      <c r="F58">
+        <v>54000</v>
+      </c>
+      <c r="G58">
+        <v>1180</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="2"/>
+        <v>1266.949152542373</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>56</v>
       </c>
       <c r="B59" s="1">
+        <f t="shared" si="0"/>
+        <v>29820000</v>
+      </c>
+      <c r="C59" s="1">
         <f t="shared" si="1"/>
-        <v>220342842.91323552</v>
-      </c>
-      <c r="C59" s="1">
-        <f t="shared" si="0"/>
         <v>560000</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="2"/>
-        <v>219782842.91323552</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>31097000.000000004</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="4"/>
+        <v>1550000</v>
+      </c>
+      <c r="F59">
+        <v>55000</v>
+      </c>
+      <c r="G59">
+        <v>1200</v>
+      </c>
+      <c r="H59" s="1">
+        <f t="shared" si="2"/>
+        <v>1291.6666666666667</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>57</v>
       </c>
       <c r="B60" s="1">
+        <f t="shared" si="0"/>
+        <v>31426000</v>
+      </c>
+      <c r="C60" s="1">
         <f t="shared" si="1"/>
-        <v>242947127.20455909</v>
-      </c>
-      <c r="C60" s="1">
-        <f t="shared" si="0"/>
         <v>570000</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="2"/>
-        <v>242377127.20455909</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>32802000.000000004</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="4"/>
+        <v>1606000</v>
+      </c>
+      <c r="F60">
+        <v>56000</v>
+      </c>
+      <c r="G60">
+        <v>1220</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" si="2"/>
+        <v>1316.3934426229507</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>58</v>
       </c>
       <c r="B61" s="1">
+        <f t="shared" si="0"/>
+        <v>33089000</v>
+      </c>
+      <c r="C61" s="1">
         <f t="shared" si="1"/>
-        <v>267821839.92501503</v>
-      </c>
-      <c r="C61" s="1">
-        <f t="shared" si="0"/>
         <v>580000</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="2"/>
-        <v>267241839.92501503</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>34568600</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="4"/>
+        <v>1663000</v>
+      </c>
+      <c r="F61">
+        <v>57000</v>
+      </c>
+      <c r="G61">
+        <v>1240</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" si="2"/>
+        <v>1341.1290322580646</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>59</v>
       </c>
       <c r="B62" s="1">
+        <f t="shared" si="0"/>
+        <v>34810000</v>
+      </c>
+      <c r="C62" s="1">
         <f t="shared" si="1"/>
-        <v>295194023.91751653</v>
-      </c>
-      <c r="C62" s="1">
-        <f t="shared" si="0"/>
         <v>590000</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="2"/>
-        <v>294604023.91751653</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>36397900</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="4"/>
+        <v>1721000</v>
+      </c>
+      <c r="F62">
+        <v>58000</v>
+      </c>
+      <c r="G62">
+        <v>1260</v>
+      </c>
+      <c r="H62" s="1">
+        <f t="shared" si="2"/>
+        <v>1365.8730158730159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>60</v>
       </c>
       <c r="B63" s="1">
+        <f t="shared" si="0"/>
+        <v>36590000</v>
+      </c>
+      <c r="C63" s="1">
         <f t="shared" si="1"/>
-        <v>325313426.30926824</v>
-      </c>
-      <c r="C63" s="1">
-        <f t="shared" si="0"/>
         <v>600000</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="2"/>
-        <v>324713426.30926824</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>38291000</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="4"/>
+        <v>1780000</v>
+      </c>
+      <c r="F63">
+        <v>59000</v>
+      </c>
+      <c r="G63">
+        <v>1280</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" si="2"/>
+        <v>1390.625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>61</v>
       </c>
       <c r="B64" s="1">
+        <f t="shared" si="0"/>
+        <v>38430000</v>
+      </c>
+      <c r="C64" s="1">
         <f t="shared" si="1"/>
-        <v>358454768.94019508</v>
-      </c>
-      <c r="C64" s="1">
-        <f t="shared" si="0"/>
         <v>610000</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="2"/>
-        <v>357844768.94019508</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>40249000</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="4"/>
+        <v>1840000</v>
+      </c>
+      <c r="F64">
+        <v>60000</v>
+      </c>
+      <c r="G64">
+        <v>1300</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="2"/>
+        <v>1415.3846153846155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>62</v>
       </c>
       <c r="B65" s="1">
+        <f t="shared" si="0"/>
+        <v>40331000</v>
+      </c>
+      <c r="C65" s="1">
         <f t="shared" si="1"/>
-        <v>394920245.83421463</v>
-      </c>
-      <c r="C65" s="1">
-        <f t="shared" si="0"/>
         <v>620000</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="2"/>
-        <v>394300245.83421463</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>42273000</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="4"/>
+        <v>1901000</v>
+      </c>
+      <c r="F65">
+        <v>61000</v>
+      </c>
+      <c r="G65">
+        <v>1320</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="2"/>
+        <v>1440.1515151515152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>63</v>
       </c>
       <c r="B66" s="1">
+        <f t="shared" si="0"/>
+        <v>42294000</v>
+      </c>
+      <c r="C66" s="1">
         <f t="shared" si="1"/>
-        <v>435042270.4176361</v>
-      </c>
-      <c r="C66" s="1">
-        <f t="shared" si="0"/>
         <v>630000</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="2"/>
-        <v>434412270.4176361</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>44364100</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="4"/>
+        <v>1963000</v>
+      </c>
+      <c r="F66">
+        <v>62000</v>
+      </c>
+      <c r="G66">
+        <v>1340</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" si="2"/>
+        <v>1464.9253731343283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>64</v>
       </c>
       <c r="B67" s="1">
+        <f t="shared" si="0"/>
+        <v>44320000</v>
+      </c>
+      <c r="C67" s="1">
         <f t="shared" si="1"/>
-        <v>479186497.45939976</v>
-      </c>
-      <c r="C67" s="1">
-        <f t="shared" si="0"/>
         <v>640000</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="2"/>
-        <v>478546497.45939976</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>46523400.000000007</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" si="4"/>
+        <v>2026000</v>
+      </c>
+      <c r="F67">
+        <v>63000</v>
+      </c>
+      <c r="G67">
+        <v>1360</v>
+      </c>
+      <c r="H67" s="1">
+        <f t="shared" si="2"/>
+        <v>1489.7058823529412</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>65</v>
       </c>
       <c r="B68" s="1">
+        <f t="shared" si="0"/>
+        <v>46410000</v>
+      </c>
+      <c r="C68" s="1">
         <f t="shared" si="1"/>
-        <v>527755147.20533979</v>
-      </c>
-      <c r="C68" s="1">
-        <f t="shared" si="0"/>
         <v>650000</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="2"/>
-        <v>527105147.20533979</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>48752000.000000007</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="4"/>
+        <v>2090000</v>
+      </c>
+      <c r="F68">
+        <v>64000</v>
+      </c>
+      <c r="G68">
+        <v>1380</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="shared" si="2"/>
+        <v>1514.4927536231885</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>66</v>
       </c>
       <c r="B69" s="1">
-        <f t="shared" ref="B69:B103" si="3">C69+D69</f>
-        <v>581190661.92587376</v>
+        <f t="shared" ref="B69:B103" si="5">B68+E69</f>
+        <v>48565000</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" ref="C69:C103" si="4">C68+$C$2</f>
+        <f t="shared" ref="C69:C103" si="6">C68+$C$2</f>
         <v>660000</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="2"/>
-        <v>580530661.92587376</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>51051000.000000007</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="4"/>
+        <v>2155000</v>
+      </c>
+      <c r="F69">
+        <v>65000</v>
+      </c>
+      <c r="G69">
+        <v>1400</v>
+      </c>
+      <c r="H69" s="1">
+        <f t="shared" ref="H69:H103" si="7">E69/G69</f>
+        <v>1539.2857142857142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>67</v>
       </c>
       <c r="B70" s="1">
-        <f t="shared" si="3"/>
-        <v>639979728.11846113</v>
+        <f t="shared" si="5"/>
+        <v>50786000</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>670000</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D103" si="5">B69*1.1</f>
-        <v>639309728.11846113</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D70:D103" si="8">B69*1.1</f>
+        <v>53421500.000000007</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" ref="E70:E103" si="9">E69+F70</f>
+        <v>2221000</v>
+      </c>
+      <c r="F70">
+        <v>66000</v>
+      </c>
+      <c r="G70">
+        <v>1420</v>
+      </c>
+      <c r="H70" s="1">
+        <f t="shared" si="7"/>
+        <v>1564.0845070422536</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>68</v>
       </c>
       <c r="B71" s="1">
-        <f t="shared" si="3"/>
-        <v>704657700.93030727</v>
+        <f t="shared" si="5"/>
+        <v>53074000</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>680000</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="5"/>
-        <v>703977700.93030727</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>55864600.000000007</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="9"/>
+        <v>2288000</v>
+      </c>
+      <c r="F71">
+        <v>67000</v>
+      </c>
+      <c r="G71">
+        <v>1440</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" si="7"/>
+        <v>1588.8888888888889</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>69</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" si="3"/>
-        <v>775813471.02333808</v>
+        <f t="shared" si="5"/>
+        <v>55430000</v>
       </c>
       <c r="C72" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>690000</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="5"/>
-        <v>775123471.02333808</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>58381400.000000007</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="9"/>
+        <v>2356000</v>
+      </c>
+      <c r="F72">
+        <v>68000</v>
+      </c>
+      <c r="G72">
+        <v>1460</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="7"/>
+        <v>1613.6986301369864</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>70</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="3"/>
-        <v>854094818.12567198</v>
+        <f t="shared" si="5"/>
+        <v>57855000</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>700000</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="5"/>
-        <v>853394818.12567198</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>60973000.000000007</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="9"/>
+        <v>2425000</v>
+      </c>
+      <c r="F73">
+        <v>69000</v>
+      </c>
+      <c r="G73">
+        <v>1480</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="7"/>
+        <v>1638.5135135135135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>71</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="3"/>
-        <v>940214299.93823922</v>
+        <f t="shared" si="5"/>
+        <v>60350000</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>710000</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="5"/>
-        <v>939504299.93823922</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>63640500.000000007</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="9"/>
+        <v>2495000</v>
+      </c>
+      <c r="F74">
+        <v>70000</v>
+      </c>
+      <c r="G74">
+        <v>1500</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="7"/>
+        <v>1663.3333333333333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>72</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" si="3"/>
-        <v>1034955729.9320632</v>
+        <f t="shared" si="5"/>
+        <v>62916000</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>720000</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="5"/>
-        <v>1034235729.9320632</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>66385000.000000007</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="9"/>
+        <v>2566000</v>
+      </c>
+      <c r="F75">
+        <v>71000</v>
+      </c>
+      <c r="G75">
+        <v>1520</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="7"/>
+        <v>1688.1578947368421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>73</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="3"/>
-        <v>1139181302.9252696</v>
+        <f t="shared" si="5"/>
+        <v>65554000</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>730000</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="5"/>
-        <v>1138451302.9252696</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>69207600</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="9"/>
+        <v>2638000</v>
+      </c>
+      <c r="F76">
+        <v>72000</v>
+      </c>
+      <c r="G76">
+        <v>1540</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="7"/>
+        <v>1712.987012987013</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>74</v>
       </c>
       <c r="B77" s="1">
-        <f t="shared" si="3"/>
-        <v>1253839433.2177966</v>
+        <f t="shared" si="5"/>
+        <v>68265000</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>740000</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="5"/>
-        <v>1253099433.2177966</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>72109400</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="9"/>
+        <v>2711000</v>
+      </c>
+      <c r="F77">
+        <v>73000</v>
+      </c>
+      <c r="G77">
+        <v>1560</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="7"/>
+        <v>1737.8205128205129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>75</v>
       </c>
       <c r="B78" s="1">
-        <f t="shared" si="3"/>
-        <v>1379973376.5395763</v>
+        <f t="shared" si="5"/>
+        <v>71050000</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>750000</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="5"/>
-        <v>1379223376.5395763</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>75091500</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="9"/>
+        <v>2785000</v>
+      </c>
+      <c r="F78">
+        <v>74000</v>
+      </c>
+      <c r="G78">
+        <v>1580</v>
+      </c>
+      <c r="H78" s="1">
+        <f t="shared" si="7"/>
+        <v>1762.6582278481012</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>76</v>
       </c>
       <c r="B79" s="1">
-        <f t="shared" si="3"/>
-        <v>1518730714.1935341</v>
+        <f t="shared" si="5"/>
+        <v>73910000</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>760000</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="5"/>
-        <v>1517970714.1935341</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>78155000</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="9"/>
+        <v>2860000</v>
+      </c>
+      <c r="F79">
+        <v>75000</v>
+      </c>
+      <c r="G79">
+        <v>1600</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" si="7"/>
+        <v>1787.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>77</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" si="3"/>
-        <v>1671373785.6128876</v>
+        <f t="shared" si="5"/>
+        <v>76846000</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>770000</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="5"/>
-        <v>1670603785.6128876</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>81301000</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="9"/>
+        <v>2936000</v>
+      </c>
+      <c r="F80">
+        <v>76000</v>
+      </c>
+      <c r="G80">
+        <v>1620</v>
+      </c>
+      <c r="H80" s="1">
+        <f t="shared" si="7"/>
+        <v>1812.3456790123457</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>78</v>
       </c>
       <c r="B81" s="1">
-        <f t="shared" si="3"/>
-        <v>1839291164.1741765</v>
+        <f t="shared" si="5"/>
+        <v>79859000</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>780000</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="5"/>
-        <v>1838511164.1741765</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>84530600</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="9"/>
+        <v>3013000</v>
+      </c>
+      <c r="F81">
+        <v>77000</v>
+      </c>
+      <c r="G81">
+        <v>1640</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" si="7"/>
+        <v>1837.1951219512196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>79</v>
       </c>
       <c r="B82" s="1">
-        <f t="shared" si="3"/>
-        <v>2024010280.5915942</v>
+        <f t="shared" si="5"/>
+        <v>82950000</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>790000</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="5"/>
-        <v>2023220280.5915942</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>87844900</v>
+      </c>
+      <c r="E82" s="1">
+        <f t="shared" si="9"/>
+        <v>3091000</v>
+      </c>
+      <c r="F82">
+        <v>78000</v>
+      </c>
+      <c r="G82">
+        <v>1660</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="7"/>
+        <v>1862.0481927710844</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>80</v>
       </c>
       <c r="B83" s="1">
-        <f t="shared" si="3"/>
-        <v>2227211308.650754</v>
+        <f t="shared" si="5"/>
+        <v>86120000</v>
       </c>
       <c r="C83" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>800000</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="5"/>
-        <v>2226411308.650754</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>91245000</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="9"/>
+        <v>3170000</v>
+      </c>
+      <c r="F83">
+        <v>79000</v>
+      </c>
+      <c r="G83">
+        <v>1680</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="7"/>
+        <v>1886.9047619047619</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>81</v>
       </c>
       <c r="B84" s="1">
-        <f t="shared" si="3"/>
-        <v>2450742439.5158296</v>
+        <f t="shared" si="5"/>
+        <v>89370000</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>810000</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="5"/>
-        <v>2449932439.5158296</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>94732000.000000015</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="9"/>
+        <v>3250000</v>
+      </c>
+      <c r="F84">
+        <v>80000</v>
+      </c>
+      <c r="G84">
+        <v>1700</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="7"/>
+        <v>1911.7647058823529</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>82</v>
       </c>
       <c r="B85" s="1">
-        <f t="shared" si="3"/>
-        <v>2696636683.4674129</v>
+        <f t="shared" si="5"/>
+        <v>92701000</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>820000</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="5"/>
-        <v>2695816683.4674129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>98307000.000000015</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="9"/>
+        <v>3331000</v>
+      </c>
+      <c r="F85">
+        <v>81000</v>
+      </c>
+      <c r="G85">
+        <v>1720</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="7"/>
+        <v>1936.6279069767443</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>83</v>
       </c>
       <c r="B86" s="1">
-        <f t="shared" si="3"/>
-        <v>2967130351.8141546</v>
+        <f t="shared" si="5"/>
+        <v>96114000</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>830000</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="5"/>
-        <v>2966300351.8141546</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>101971100.00000001</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="9"/>
+        <v>3413000</v>
+      </c>
+      <c r="F86">
+        <v>82000</v>
+      </c>
+      <c r="G86">
+        <v>1740</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="7"/>
+        <v>1961.4942528735633</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>84</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="3"/>
-        <v>3264683386.9955702</v>
+        <f t="shared" si="5"/>
+        <v>99610000</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>840000</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="5"/>
-        <v>3263843386.9955702</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>105725400.00000001</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="9"/>
+        <v>3496000</v>
+      </c>
+      <c r="F87">
+        <v>83000</v>
+      </c>
+      <c r="G87">
+        <v>1760</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="7"/>
+        <v>1986.3636363636363</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>85</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="3"/>
-        <v>3592001725.6951275</v>
+        <f t="shared" si="5"/>
+        <v>103190000</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>850000</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="5"/>
-        <v>3591151725.6951275</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>109571000.00000001</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="9"/>
+        <v>3580000</v>
+      </c>
+      <c r="F88">
+        <v>84000</v>
+      </c>
+      <c r="G88">
+        <v>1780</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="7"/>
+        <v>2011.2359550561798</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>86</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="3"/>
-        <v>3952061898.2646403</v>
+        <f t="shared" si="5"/>
+        <v>106855000</v>
       </c>
       <c r="C89" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>860000</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="5"/>
-        <v>3951201898.2646403</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>113509000.00000001</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="9"/>
+        <v>3665000</v>
+      </c>
+      <c r="F89">
+        <v>85000</v>
+      </c>
+      <c r="G89">
+        <v>1800</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="7"/>
+        <v>2036.1111111111111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>87</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="3"/>
-        <v>4348138088.0911045</v>
+        <f t="shared" si="5"/>
+        <v>110606000</v>
       </c>
       <c r="C90" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>870000</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="5"/>
-        <v>4347268088.0911045</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>117540500.00000001</v>
+      </c>
+      <c r="E90" s="1">
+        <f t="shared" si="9"/>
+        <v>3751000</v>
+      </c>
+      <c r="F90">
+        <v>86000</v>
+      </c>
+      <c r="G90">
+        <v>1820</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="7"/>
+        <v>2060.9890109890111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>88</v>
       </c>
       <c r="B91" s="1">
-        <f t="shared" si="3"/>
-        <v>4783831896.9002151</v>
+        <f t="shared" si="5"/>
+        <v>114444000</v>
       </c>
       <c r="C91" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>880000</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="5"/>
-        <v>4782951896.9002151</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>121666600.00000001</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="9"/>
+        <v>3838000</v>
+      </c>
+      <c r="F91">
+        <v>87000</v>
+      </c>
+      <c r="G91">
+        <v>1840</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="7"/>
+        <v>2085.8695652173915</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>89</v>
       </c>
       <c r="B92" s="1">
-        <f t="shared" si="3"/>
-        <v>5263105086.5902367</v>
+        <f t="shared" si="5"/>
+        <v>118370000</v>
       </c>
       <c r="C92" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>890000</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="5"/>
-        <v>5262215086.5902367</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>125888400.00000001</v>
+      </c>
+      <c r="E92" s="1">
+        <f t="shared" si="9"/>
+        <v>3926000</v>
+      </c>
+      <c r="F92">
+        <v>88000</v>
+      </c>
+      <c r="G92">
+        <v>1860</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" si="7"/>
+        <v>2110.7526881720432</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>90</v>
       </c>
       <c r="B93" s="1">
-        <f t="shared" si="3"/>
-        <v>5790315595.2492609</v>
+        <f t="shared" si="5"/>
+        <v>122385000</v>
       </c>
       <c r="C93" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>900000</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="5"/>
-        <v>5789415595.2492609</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>130207000.00000001</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" si="9"/>
+        <v>4015000</v>
+      </c>
+      <c r="F93">
+        <v>89000</v>
+      </c>
+      <c r="G93">
+        <v>1880</v>
+      </c>
+      <c r="H93" s="1">
+        <f t="shared" si="7"/>
+        <v>2135.6382978723404</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>91</v>
       </c>
       <c r="B94" s="1">
-        <f t="shared" si="3"/>
-        <v>6370257154.7741871</v>
+        <f t="shared" si="5"/>
+        <v>126490000</v>
       </c>
       <c r="C94" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>910000</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="5"/>
-        <v>6369347154.7741871</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>134623500</v>
+      </c>
+      <c r="E94" s="1">
+        <f t="shared" si="9"/>
+        <v>4105000</v>
+      </c>
+      <c r="F94">
+        <v>90000</v>
+      </c>
+      <c r="G94">
+        <v>1900</v>
+      </c>
+      <c r="H94" s="1">
+        <f t="shared" si="7"/>
+        <v>2160.5263157894738</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>92</v>
       </c>
       <c r="B95" s="1">
-        <f t="shared" si="3"/>
-        <v>7008202870.251606</v>
+        <f t="shared" si="5"/>
+        <v>130686000</v>
       </c>
       <c r="C95" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>920000</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="5"/>
-        <v>7007282870.251606</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>139139000</v>
+      </c>
+      <c r="E95" s="1">
+        <f t="shared" si="9"/>
+        <v>4196000</v>
+      </c>
+      <c r="F95">
+        <v>91000</v>
+      </c>
+      <c r="G95">
+        <v>1920</v>
+      </c>
+      <c r="H95" s="1">
+        <f t="shared" si="7"/>
+        <v>2185.4166666666665</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>93</v>
       </c>
       <c r="B96" s="1">
-        <f t="shared" si="3"/>
-        <v>7709953157.2767668</v>
+        <f t="shared" si="5"/>
+        <v>134974000</v>
       </c>
       <c r="C96" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>930000</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="5"/>
-        <v>7709023157.2767668</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>143754600</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" si="9"/>
+        <v>4288000</v>
+      </c>
+      <c r="F96">
+        <v>92000</v>
+      </c>
+      <c r="G96">
+        <v>1940</v>
+      </c>
+      <c r="H96" s="1">
+        <f t="shared" si="7"/>
+        <v>2210.3092783505153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>94</v>
       </c>
       <c r="B97" s="1">
-        <f t="shared" si="3"/>
-        <v>8481888473.0044441</v>
+        <f t="shared" si="5"/>
+        <v>139355000</v>
       </c>
       <c r="C97" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>940000</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="5"/>
-        <v>8480948473.0044441</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>148471400</v>
+      </c>
+      <c r="E97" s="1">
+        <f t="shared" si="9"/>
+        <v>4381000</v>
+      </c>
+      <c r="F97">
+        <v>93000</v>
+      </c>
+      <c r="G97">
+        <v>1960</v>
+      </c>
+      <c r="H97" s="1">
+        <f t="shared" si="7"/>
+        <v>2235.204081632653</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>95</v>
       </c>
       <c r="B98" s="1">
-        <f t="shared" si="3"/>
-        <v>9331027320.3048897</v>
+        <f t="shared" si="5"/>
+        <v>143830000</v>
       </c>
       <c r="C98" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>950000</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="5"/>
-        <v>9330077320.3048897</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>153290500</v>
+      </c>
+      <c r="E98" s="1">
+        <f t="shared" si="9"/>
+        <v>4475000</v>
+      </c>
+      <c r="F98">
+        <v>94000</v>
+      </c>
+      <c r="G98">
+        <v>1980</v>
+      </c>
+      <c r="H98" s="1">
+        <f t="shared" si="7"/>
+        <v>2260.1010101010102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>96</v>
       </c>
       <c r="B99" s="1">
-        <f t="shared" si="3"/>
-        <v>10265090052.335379</v>
+        <f t="shared" si="5"/>
+        <v>148400000</v>
       </c>
       <c r="C99" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>960000</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="5"/>
-        <v>10264130052.335379</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>158213000</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="9"/>
+        <v>4570000</v>
+      </c>
+      <c r="F99">
+        <v>95000</v>
+      </c>
+      <c r="G99">
+        <v>2000</v>
+      </c>
+      <c r="H99" s="1">
+        <f t="shared" si="7"/>
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>97</v>
       </c>
       <c r="B100" s="1">
-        <f t="shared" si="3"/>
-        <v>11292569057.568918</v>
+        <f t="shared" si="5"/>
+        <v>153066000</v>
       </c>
       <c r="C100" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>970000</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="5"/>
-        <v>11291599057.568918</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>163240000</v>
+      </c>
+      <c r="E100" s="1">
+        <f t="shared" si="9"/>
+        <v>4666000</v>
+      </c>
+      <c r="F100">
+        <v>96000</v>
+      </c>
+      <c r="G100">
+        <v>2020</v>
+      </c>
+      <c r="H100" s="1">
+        <f t="shared" si="7"/>
+        <v>2309.90099009901</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>98</v>
       </c>
       <c r="B101" s="1">
-        <f t="shared" si="3"/>
-        <v>12422805963.325811</v>
+        <f t="shared" si="5"/>
+        <v>157829000</v>
       </c>
       <c r="C101" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>980000</v>
       </c>
       <c r="D101" s="1">
-        <f t="shared" si="5"/>
-        <v>12421825963.325811</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>168372600</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" si="9"/>
+        <v>4763000</v>
+      </c>
+      <c r="F101">
+        <v>97000</v>
+      </c>
+      <c r="G101">
+        <v>2040</v>
+      </c>
+      <c r="H101" s="1">
+        <f t="shared" si="7"/>
+        <v>2334.8039215686276</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>99</v>
       </c>
       <c r="B102" s="1">
-        <f t="shared" si="3"/>
-        <v>13666076559.658394</v>
+        <f t="shared" si="5"/>
+        <v>162690000</v>
       </c>
       <c r="C102" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>990000</v>
       </c>
       <c r="D102" s="1">
-        <f t="shared" si="5"/>
-        <v>13665086559.658394</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>173611900</v>
+      </c>
+      <c r="E102" s="1">
+        <f t="shared" si="9"/>
+        <v>4861000</v>
+      </c>
+      <c r="F102">
+        <v>98000</v>
+      </c>
+      <c r="G102">
+        <v>2060</v>
+      </c>
+      <c r="H102" s="1">
+        <f t="shared" si="7"/>
+        <v>2359.7087378640776</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>100</v>
       </c>
       <c r="B103" s="1">
-        <f t="shared" si="3"/>
-        <v>15033684215.624235</v>
+        <f t="shared" si="5"/>
+        <v>167650000</v>
       </c>
       <c r="C103" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1000000</v>
       </c>
       <c r="D103" s="1">
-        <f t="shared" si="5"/>
-        <v>15032684215.624235</v>
+        <f t="shared" si="8"/>
+        <v>178959000</v>
+      </c>
+      <c r="E103" s="1">
+        <f t="shared" si="9"/>
+        <v>4960000</v>
+      </c>
+      <c r="F103">
+        <v>99000</v>
+      </c>
+      <c r="G103">
+        <v>2080</v>
+      </c>
+      <c r="H103" s="1">
+        <f t="shared" si="7"/>
+        <v>2384.6153846153848</v>
       </c>
     </row>
   </sheetData>
@@ -2156,7 +3579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2169,12 +3592,12 @@
   <sheetData>
     <row r="1" spans="2:74" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="2:74" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>

</xml_diff>